<commit_message>
failed new final Banner Slicer | commit b4 editing table colors
</commit_message>
<xml_diff>
--- a/Excel Files/Banner and BU Dimension.xlsx
+++ b/Excel Files/Banner and BU Dimension.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_ Rob Repo\PMO-Dashboard\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlysam\Documents\PMO Final Folder\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974CFC3B-62AD-42D7-98E1-FE1980F029AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4065" yWindow="4065" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4070" yWindow="4070" windowWidth="21600" windowHeight="11390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -124,7 +123,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -480,18 +479,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,7 +500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -507,7 +508,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -515,7 +516,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -523,7 +524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -531,7 +532,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -539,7 +540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -547,7 +548,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -555,7 +556,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -563,7 +564,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -571,7 +572,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -579,7 +580,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -587,7 +588,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -595,7 +596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -603,7 +604,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -611,7 +612,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -619,7 +620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -627,7 +628,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -635,7 +636,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -643,7 +644,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -651,7 +652,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -659,7 +660,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -667,7 +668,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -675,7 +676,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -685,5 +686,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>